<commit_message>
floorButtons & person disapearing
floor buttons work well.
cool person disapearing on their floors
</commit_message>
<xml_diff>
--- a/Assets/TODO/ELEVATOR_TODO.xlsx
+++ b/Assets/TODO/ELEVATOR_TODO.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1712141483" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1712141483" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1712141483" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1712141483"/>
+      <pm:revision xmlns:pm="smNativeData" day="1712233904" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1712233904" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1712233904" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1712233904"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <r>
       <rPr>
@@ -36,7 +36,7 @@
         <u val="single"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1712141483" ulstyle="single">
+            <pm:charSpec xmlns:pm="smNativeData" id="1712233904" ulstyle="single">
               <pm:latin face="Arial" sz="260" weight="normal" i="0"/>
               <pm:cs/>
               <pm:ea/>
@@ -57,7 +57,7 @@
         <color rgb="FFCC4125"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1712141483" fgClr="CC4125">
+            <pm:charSpec xmlns:pm="smNativeData" id="1712233904" fgClr="CC4125">
               <pm:latin face="Arial" sz="260" weight="bold" i="0"/>
               <pm:cs/>
               <pm:ea/>
@@ -78,7 +78,7 @@
         <color rgb="FF000000"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1712141483" fgClr="000000">
+            <pm:charSpec xmlns:pm="smNativeData" id="1712233904" fgClr="000000">
               <pm:latin face="Arial" sz="260" weight="normal" i="0"/>
               <pm:cs/>
               <pm:ea/>
@@ -131,12 +131,15 @@
   <si>
     <t>настроить вместимость лифта, для ограничения количества человек в нём</t>
   </si>
+  <si>
+    <t>сделать стартовое меню с возможностью установки основыных параметров игры</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;₽&quot;;\-#,##0\ &quot;₽&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;₽&quot;;[Red]\-#,##0\ &quot;₽&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;₽&quot;;\-#,##0.00\ &quot;₽&quot;"/>
@@ -146,8 +149,9 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="DD.MM.YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <charset val="204"/>
@@ -156,7 +160,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1712141483" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1712233904" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -173,7 +177,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1712141483" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1712233904" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="260" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -191,8 +195,25 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1712141483" fgClr="CC4125" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1712233904" fgClr="CC4125" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="260" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="200" lang="default"/>
+            <pm:ea face="SimSun" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <strike/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1712233904" ulstyle="none" strike="1" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
           </pm:charSpec>
@@ -213,7 +234,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1712141483" type="1" fgLvl="100" fgClr="00E06666" bgLvl="0" bgClr="00E06666"/>
+            <pm:shade xmlns:pm="smNativeData" id="1712233904" type="1" fgLvl="100" fgClr="00E06666" bgLvl="0" bgClr="00E06666"/>
           </ext>
         </extLst>
       </patternFill>
@@ -224,7 +245,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1712141483" type="1" fgLvl="100" fgClr="00B6D7A8" bgLvl="0" bgClr="00B6D7A8"/>
+            <pm:shade xmlns:pm="smNativeData" id="1712233904" type="1" fgLvl="100" fgClr="00B6D7A8" bgLvl="0" bgClr="00B6D7A8"/>
           </ext>
         </extLst>
       </patternFill>
@@ -235,7 +256,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1712141483" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1712233904" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -257,7 +278,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1712141483"/>
+          <pm:border xmlns:pm="smNativeData" id="1712233904"/>
         </ext>
       </extLst>
     </border>
@@ -276,7 +297,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1712141483"/>
+          <pm:border xmlns:pm="smNativeData" id="1712233904"/>
         </ext>
       </extLst>
     </border>
@@ -295,7 +316,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1712141483"/>
+          <pm:border xmlns:pm="smNativeData" id="1712233904"/>
         </ext>
       </extLst>
     </border>
@@ -314,7 +335,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1712141483"/>
+          <pm:border xmlns:pm="smNativeData" id="1712233904"/>
         </ext>
       </extLst>
     </border>
@@ -322,15 +343,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -338,10 +364,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1712141483" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1712233904" count="1">
         <pm:charStyle name="Обычный" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1712141483" count="3">
+      <pm:colors xmlns:pm="smNativeData" id="1712233904" count="3">
         <pm:color name="Цвет 24" rgb="E06666"/>
         <pm:color name="Цвет 25" rgb="B6D7A8"/>
         <pm:color name="Цвет 26" rgb="CC4125"/>
@@ -610,10 +636,10 @@
   <sheetPr>
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="11" defaultColWidth="12.630631" defaultRowHeight="15.75" customHeight="1"/>
@@ -648,17 +674,17 @@
       <c r="A4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3" t="n">
+      <c r="C4" s="6"/>
+      <c r="D4" s="7" t="n">
         <v>45380</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="7" t="n">
         <v>45381</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -684,7 +710,7 @@
       <c r="B6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="3" t="n">
         <v>45380</v>
       </c>
@@ -699,7 +725,7 @@
       <c r="B7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="3" t="n">
         <v>45383</v>
       </c>
@@ -711,29 +737,35 @@
       <c r="A8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3" t="n">
+      <c r="C8" s="6"/>
+      <c r="D8" s="7" t="n">
         <v>45383</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="10" t="n">
+        <v>45385</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="B9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3" t="n">
+      <c r="C9" s="6"/>
+      <c r="D9" s="7" t="n">
         <v>45383</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="8" t="n">
+        <v>45386</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -774,7 +806,7 @@
       <c r="B12" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="3" t="n">
         <v>45385</v>
       </c>
@@ -787,14 +819,29 @@
         <v>0</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C13" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="3" t="n">
         <v>45385</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="3" t="n">
+        <v>45386</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -804,7 +851,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1712141483" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1712233904" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -813,16 +860,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1712141483" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1712141483" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1712141483" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1712141483" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1712233904" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1712233904" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1712233904" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1712233904" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1712141483" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1712233904" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
replace elevator move logic lo elGO
</commit_message>
<xml_diff>
--- a/Assets/TODO/ELEVATOR_TODO.xlsx
+++ b/Assets/TODO/ELEVATOR_TODO.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1712919979" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1712919979" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1712919979" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1712919979"/>
+      <pm:revision xmlns:pm="smNativeData" day="1712927618" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1712927618" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1712927618" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1712927618"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <r>
       <rPr>
@@ -36,7 +36,7 @@
         <u val="single"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1712919979" ulstyle="single">
+            <pm:charSpec xmlns:pm="smNativeData" id="1712927618" ulstyle="single">
               <pm:latin face="Arial" sz="260" weight="normal" i="0"/>
               <pm:cs/>
               <pm:ea/>
@@ -58,7 +58,7 @@
         <color rgb="FFCC4125"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1712919979" fgClr="CC4125" ulstyle="none">
+            <pm:charSpec xmlns:pm="smNativeData" id="1712927618" fgClr="CC4125" ulstyle="none">
               <pm:latin face="Arial" sz="260" weight="bold" i="0"/>
               <pm:cs/>
               <pm:ea/>
@@ -79,7 +79,7 @@
         <color rgb="FF000000"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:charSpec xmlns:pm="smNativeData" id="1712919979" fgClr="000000">
+            <pm:charSpec xmlns:pm="smNativeData" id="1712927618" fgClr="000000">
               <pm:latin face="Arial" sz="260" weight="normal" i="0"/>
               <pm:cs/>
               <pm:ea/>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>сделать стартовое меню с возможностью установки основыных параметров игры</t>
+  </si>
+  <si>
+    <t>переместить MainMenu и Boot в project context</t>
+  </si>
+  <si>
+    <t>реализовать Event Bus</t>
   </si>
 </sst>
 </file>
@@ -161,7 +167,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1712919979" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1712927618" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -178,7 +184,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1712919979" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1712927618" ulstyle="single" kern="1">
             <pm:latin face="Arial" sz="260" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -195,7 +201,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1712919979" ulstyle="none" strike="1" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1712927618" ulstyle="none" strike="1" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -211,7 +217,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1712919979" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1712927618" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Arial" sz="200" lang="default"/>
             <pm:ea face="Arial" sz="200" lang="default"/>
@@ -228,7 +234,7 @@
       <sz val="13"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1712919979" fgClr="CC4125" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1712927618" fgClr="CC4125" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="260" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -244,7 +250,7 @@
       <sz val="13"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1712919979" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1712927618" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="260" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -253,7 +259,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,7 +272,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1712919979" type="1" fgLvl="100" fgClr="00E06666" bgLvl="0" bgClr="00E06666"/>
+            <pm:shade xmlns:pm="smNativeData" id="1712927618" type="1" fgLvl="100" fgClr="00E06666" bgLvl="0" bgClr="00E06666"/>
           </ext>
         </extLst>
       </patternFill>
@@ -277,13 +283,24 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1712919979" type="1" fgLvl="100" fgClr="00B6D7A8" bgLvl="0" bgClr="00B6D7A8"/>
+            <pm:shade xmlns:pm="smNativeData" id="1712927618" type="1" fgLvl="100" fgClr="00B6D7A8" bgLvl="0" bgClr="00B6D7A8"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1712927618" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -299,7 +316,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1712919979"/>
+          <pm:border xmlns:pm="smNativeData" id="1712927618"/>
         </ext>
       </extLst>
     </border>
@@ -318,7 +335,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1712919979"/>
+          <pm:border xmlns:pm="smNativeData" id="1712927618"/>
         </ext>
       </extLst>
     </border>
@@ -337,7 +354,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1712919979"/>
+          <pm:border xmlns:pm="smNativeData" id="1712927618"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1712927618"/>
         </ext>
       </extLst>
     </border>
@@ -345,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -361,6 +397,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -368,10 +405,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1712919979" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1712927618" count="1">
         <pm:charStyle name="Обычный" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1712919979" count="3">
+      <pm:colors xmlns:pm="smNativeData" id="1712927618" count="3">
         <pm:color name="Цвет 24" rgb="E06666"/>
         <pm:color name="Цвет 25" rgb="B6D7A8"/>
         <pm:color name="Цвет 26" rgb="CC4125"/>
@@ -640,10 +677,10 @@
   <sheetPr>
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:F12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="11" defaultColWidth="12.630631" defaultRowHeight="15.75" customHeight="1"/>
@@ -844,9 +881,41 @@
       <c r="D14" s="12" t="n">
         <v>45386</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="13" t="n">
+        <v>45394</v>
+      </c>
       <c r="F14" s="10" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" t="n">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2" t="n">
+        <v>45394</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A16" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" t="n">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="2" t="n">
+        <v>45394</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -856,7 +925,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1712919979" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1712927618" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -865,16 +934,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1712919979" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1712919979" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1712919979" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1712919979" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1712927618" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1712927618" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1712927618" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1712927618" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1712919979" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1712927618" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>